<commit_message>
Attempting to figure out why the program is slow for certain numbers
</commit_message>
<xml_diff>
--- a/N-Queens_Prototype_Support.xlsx
+++ b/N-Queens_Prototype_Support.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Project Files\N_Queen_Solver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{384EE8D2-C205-42BA-9D06-913D10C89067}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{788C9124-12E4-4241-AD14-C910931E47D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3780" yWindow="795" windowWidth="20250" windowHeight="15480" activeTab="1" xr2:uid="{A2BBAF73-77DC-419B-BD36-C76893C774A0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{A2BBAF73-77DC-419B-BD36-C76893C774A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -771,8 +771,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E2C2ACD-CDD0-4DFC-AE98-62EA7F60ADB4}">
   <dimension ref="A1:W29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AB25" sqref="AB25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="36" x14ac:dyDescent="0.25"/>
@@ -1827,35 +1827,35 @@
         <v>0</v>
       </c>
       <c r="C19" s="13">
-        <f t="shared" ref="C19:J19" si="11">$A19+C$18</f>
+        <f>$A19+C$18</f>
         <v>1</v>
       </c>
       <c r="D19" s="15">
-        <f t="shared" si="11"/>
+        <f>$A19+D$18</f>
         <v>2</v>
       </c>
       <c r="E19" s="13">
-        <f t="shared" si="11"/>
+        <f>$A19+E$18</f>
         <v>3</v>
       </c>
       <c r="F19" s="15">
-        <f t="shared" si="11"/>
+        <f>$A19+F$18</f>
         <v>4</v>
       </c>
       <c r="G19" s="13">
-        <f t="shared" si="11"/>
+        <f>$A19+G$18</f>
         <v>5</v>
       </c>
       <c r="H19" s="15">
-        <f t="shared" si="11"/>
+        <f>$A19+H$18</f>
         <v>6</v>
       </c>
       <c r="I19" s="13">
-        <f t="shared" si="11"/>
+        <f>$A19+I$18</f>
         <v>7</v>
       </c>
       <c r="J19" s="15">
-        <f t="shared" si="11"/>
+        <f>$A19+J$18</f>
         <v>8</v>
       </c>
       <c r="K19" s="20"/>
@@ -1868,31 +1868,31 @@
         <v>0</v>
       </c>
       <c r="O19" s="12">
-        <f t="shared" ref="O19:U19" si="12">$M19+O$18</f>
+        <f>$M19+O$18</f>
         <v>1</v>
       </c>
       <c r="P19" s="16">
-        <f t="shared" si="12"/>
+        <f>$M19+P$18</f>
         <v>2</v>
       </c>
       <c r="Q19" s="12">
-        <f t="shared" si="12"/>
+        <f>$M19+Q$18</f>
         <v>3</v>
       </c>
       <c r="R19" s="16">
-        <f t="shared" si="12"/>
+        <f>$M19+R$18</f>
         <v>4</v>
       </c>
       <c r="S19" s="12">
-        <f t="shared" si="12"/>
+        <f>$M19+S$18</f>
         <v>5</v>
       </c>
       <c r="T19" s="16">
-        <f t="shared" si="12"/>
+        <f>$M19+T$18</f>
         <v>6</v>
       </c>
       <c r="U19" s="12">
-        <f t="shared" si="12"/>
+        <f>$M19+U$18</f>
         <v>7</v>
       </c>
       <c r="V19" s="20"/>
@@ -1903,39 +1903,39 @@
         <v>1</v>
       </c>
       <c r="B20" s="13">
-        <f t="shared" ref="B20:J27" si="13">$A20+B$18</f>
+        <f>$A20+B$18</f>
         <v>1</v>
       </c>
       <c r="C20" s="15">
-        <f t="shared" si="13"/>
+        <f>$A20+C$18</f>
         <v>2</v>
       </c>
       <c r="D20" s="13">
-        <f t="shared" si="13"/>
+        <f>$A20+D$18</f>
         <v>3</v>
       </c>
       <c r="E20" s="15">
-        <f t="shared" si="13"/>
+        <f>$A20+E$18</f>
         <v>4</v>
       </c>
       <c r="F20" s="13">
-        <f t="shared" si="13"/>
+        <f>$A20+F$18</f>
         <v>5</v>
       </c>
       <c r="G20" s="15">
-        <f t="shared" si="13"/>
+        <f>$A20+G$18</f>
         <v>6</v>
       </c>
       <c r="H20" s="13">
-        <f t="shared" si="13"/>
+        <f>$A20+H$18</f>
         <v>7</v>
       </c>
       <c r="I20" s="15">
-        <f t="shared" si="13"/>
+        <f>$A20+I$18</f>
         <v>8</v>
       </c>
       <c r="J20" s="13">
-        <f t="shared" si="13"/>
+        <f>$A20+J$18</f>
         <v>9</v>
       </c>
       <c r="K20" s="19">
@@ -1946,35 +1946,35 @@
         <v>1</v>
       </c>
       <c r="N20" s="12">
-        <f t="shared" ref="N20:U26" si="14">$M20+N$18</f>
+        <f>$M20+N$18</f>
         <v>1</v>
       </c>
       <c r="O20" s="16">
-        <f t="shared" si="14"/>
+        <f>$M20+O$18</f>
         <v>2</v>
       </c>
       <c r="P20" s="12">
-        <f t="shared" si="14"/>
+        <f>$M20+P$18</f>
         <v>3</v>
       </c>
       <c r="Q20" s="16">
-        <f t="shared" si="14"/>
+        <f>$M20+Q$18</f>
         <v>4</v>
       </c>
       <c r="R20" s="12">
-        <f t="shared" si="14"/>
+        <f>$M20+R$18</f>
         <v>5</v>
       </c>
       <c r="S20" s="16">
-        <f t="shared" si="14"/>
+        <f>$M20+S$18</f>
         <v>6</v>
       </c>
       <c r="T20" s="12">
-        <f t="shared" si="14"/>
+        <f>$M20+T$18</f>
         <v>7</v>
       </c>
       <c r="U20" s="16">
-        <f t="shared" si="14"/>
+        <f>$M20+U$18</f>
         <v>8</v>
       </c>
       <c r="V20" s="20">
@@ -1987,39 +1987,39 @@
         <v>2</v>
       </c>
       <c r="B21" s="15">
-        <f t="shared" si="13"/>
+        <f>$A21+B$18</f>
         <v>2</v>
       </c>
       <c r="C21" s="13">
-        <f t="shared" si="13"/>
+        <f>$A21+C$18</f>
         <v>3</v>
       </c>
       <c r="D21" s="15">
-        <f t="shared" si="13"/>
+        <f>$A21+D$18</f>
         <v>4</v>
       </c>
       <c r="E21" s="13">
-        <f t="shared" si="13"/>
+        <f>$A21+E$18</f>
         <v>5</v>
       </c>
       <c r="F21" s="15">
-        <f t="shared" si="13"/>
+        <f>$A21+F$18</f>
         <v>6</v>
       </c>
       <c r="G21" s="13">
-        <f t="shared" si="13"/>
+        <f>$A21+G$18</f>
         <v>7</v>
       </c>
       <c r="H21" s="15">
-        <f t="shared" si="13"/>
+        <f>$A21+H$18</f>
         <v>8</v>
       </c>
       <c r="I21" s="13">
-        <f t="shared" si="13"/>
+        <f>$A21+I$18</f>
         <v>9</v>
       </c>
       <c r="J21" s="15">
-        <f t="shared" si="13"/>
+        <f>$A21+J$18</f>
         <v>10</v>
       </c>
       <c r="K21" s="20">
@@ -2030,35 +2030,35 @@
         <v>2</v>
       </c>
       <c r="N21" s="16">
-        <f t="shared" si="14"/>
+        <f>$M21+N$18</f>
         <v>2</v>
       </c>
       <c r="O21" s="12">
-        <f t="shared" si="14"/>
+        <f>$M21+O$18</f>
         <v>3</v>
       </c>
       <c r="P21" s="16">
-        <f t="shared" si="14"/>
+        <f>$M21+P$18</f>
         <v>4</v>
       </c>
       <c r="Q21" s="12">
-        <f t="shared" si="14"/>
+        <f>$M21+Q$18</f>
         <v>5</v>
       </c>
       <c r="R21" s="16">
-        <f t="shared" si="14"/>
+        <f>$M21+R$18</f>
         <v>6</v>
       </c>
       <c r="S21" s="12">
-        <f t="shared" si="14"/>
+        <f>$M21+S$18</f>
         <v>7</v>
       </c>
       <c r="T21" s="16">
-        <f t="shared" si="14"/>
+        <f>$M21+T$18</f>
         <v>8</v>
       </c>
       <c r="U21" s="12">
-        <f t="shared" si="14"/>
+        <f>$M21+U$18</f>
         <v>9</v>
       </c>
       <c r="V21" s="19">
@@ -2071,39 +2071,39 @@
         <v>3</v>
       </c>
       <c r="B22" s="13">
-        <f t="shared" si="13"/>
+        <f>$A22+B$18</f>
         <v>3</v>
       </c>
       <c r="C22" s="15">
-        <f t="shared" si="13"/>
+        <f>$A22+C$18</f>
         <v>4</v>
       </c>
       <c r="D22" s="13">
-        <f t="shared" si="13"/>
+        <f>$A22+D$18</f>
         <v>5</v>
       </c>
       <c r="E22" s="15">
-        <f t="shared" si="13"/>
+        <f>$A22+E$18</f>
         <v>6</v>
       </c>
       <c r="F22" s="13">
-        <f t="shared" si="13"/>
+        <f>$A22+F$18</f>
         <v>7</v>
       </c>
       <c r="G22" s="15">
-        <f t="shared" si="13"/>
+        <f>$A22+G$18</f>
         <v>8</v>
       </c>
       <c r="H22" s="13">
-        <f t="shared" si="13"/>
+        <f>$A22+H$18</f>
         <v>9</v>
       </c>
       <c r="I22" s="15">
-        <f t="shared" si="13"/>
+        <f>$A22+I$18</f>
         <v>10</v>
       </c>
       <c r="J22" s="13">
-        <f t="shared" si="13"/>
+        <f>$A22+J$18</f>
         <v>11</v>
       </c>
       <c r="K22" s="19">
@@ -2114,35 +2114,35 @@
         <v>3</v>
       </c>
       <c r="N22" s="12">
-        <f t="shared" si="14"/>
+        <f>$M22+N$18</f>
         <v>3</v>
       </c>
       <c r="O22" s="16">
-        <f t="shared" si="14"/>
+        <f>$M22+O$18</f>
         <v>4</v>
       </c>
       <c r="P22" s="12">
-        <f t="shared" si="14"/>
+        <f>$M22+P$18</f>
         <v>5</v>
       </c>
       <c r="Q22" s="16">
-        <f t="shared" si="14"/>
+        <f>$M22+Q$18</f>
         <v>6</v>
       </c>
       <c r="R22" s="12">
-        <f t="shared" si="14"/>
+        <f>$M22+R$18</f>
         <v>7</v>
       </c>
       <c r="S22" s="16">
-        <f t="shared" si="14"/>
+        <f>$M22+S$18</f>
         <v>8</v>
       </c>
       <c r="T22" s="12">
-        <f t="shared" si="14"/>
+        <f>$M22+T$18</f>
         <v>9</v>
       </c>
       <c r="U22" s="16">
-        <f t="shared" si="14"/>
+        <f>$M22+U$18</f>
         <v>10</v>
       </c>
       <c r="V22" s="20">
@@ -2155,39 +2155,39 @@
         <v>4</v>
       </c>
       <c r="B23" s="15">
-        <f t="shared" si="13"/>
+        <f>$A23+B$18</f>
         <v>4</v>
       </c>
       <c r="C23" s="13">
-        <f t="shared" si="13"/>
+        <f>$A23+C$18</f>
         <v>5</v>
       </c>
       <c r="D23" s="15">
-        <f t="shared" si="13"/>
+        <f>$A23+D$18</f>
         <v>6</v>
       </c>
       <c r="E23" s="13">
-        <f t="shared" si="13"/>
+        <f>$A23+E$18</f>
         <v>7</v>
       </c>
       <c r="F23" s="15">
-        <f t="shared" si="13"/>
+        <f>$A23+F$18</f>
         <v>8</v>
       </c>
       <c r="G23" s="13">
-        <f t="shared" si="13"/>
+        <f>$A23+G$18</f>
         <v>9</v>
       </c>
       <c r="H23" s="15">
-        <f t="shared" si="13"/>
+        <f>$A23+H$18</f>
         <v>10</v>
       </c>
       <c r="I23" s="13">
-        <f t="shared" si="13"/>
+        <f>$A23+I$18</f>
         <v>11</v>
       </c>
       <c r="J23" s="15">
-        <f t="shared" si="13"/>
+        <f>$A23+J$18</f>
         <v>12</v>
       </c>
       <c r="K23" s="20">
@@ -2198,35 +2198,35 @@
         <v>4</v>
       </c>
       <c r="N23" s="16">
-        <f t="shared" si="14"/>
+        <f>$M23+N$18</f>
         <v>4</v>
       </c>
       <c r="O23" s="12">
-        <f t="shared" si="14"/>
+        <f>$M23+O$18</f>
         <v>5</v>
       </c>
       <c r="P23" s="16">
-        <f t="shared" si="14"/>
+        <f>$M23+P$18</f>
         <v>6</v>
       </c>
       <c r="Q23" s="12">
-        <f t="shared" si="14"/>
+        <f>$M23+Q$18</f>
         <v>7</v>
       </c>
       <c r="R23" s="16">
-        <f t="shared" si="14"/>
+        <f>$M23+R$18</f>
         <v>8</v>
       </c>
       <c r="S23" s="12">
-        <f t="shared" si="14"/>
+        <f>$M23+S$18</f>
         <v>9</v>
       </c>
       <c r="T23" s="16">
-        <f t="shared" si="14"/>
+        <f>$M23+T$18</f>
         <v>10</v>
       </c>
       <c r="U23" s="12">
-        <f t="shared" si="14"/>
+        <f>$M23+U$18</f>
         <v>11</v>
       </c>
       <c r="V23" s="19">
@@ -2239,39 +2239,39 @@
         <v>5</v>
       </c>
       <c r="B24" s="13">
-        <f t="shared" si="13"/>
+        <f>$A24+B$18</f>
         <v>5</v>
       </c>
       <c r="C24" s="15">
-        <f t="shared" si="13"/>
+        <f>$A24+C$18</f>
         <v>6</v>
       </c>
       <c r="D24" s="13">
-        <f t="shared" si="13"/>
+        <f>$A24+D$18</f>
         <v>7</v>
       </c>
       <c r="E24" s="15">
-        <f t="shared" si="13"/>
+        <f>$A24+E$18</f>
         <v>8</v>
       </c>
       <c r="F24" s="13">
-        <f t="shared" si="13"/>
+        <f>$A24+F$18</f>
         <v>9</v>
       </c>
       <c r="G24" s="15">
-        <f t="shared" si="13"/>
+        <f>$A24+G$18</f>
         <v>10</v>
       </c>
       <c r="H24" s="13">
-        <f t="shared" si="13"/>
+        <f>$A24+H$18</f>
         <v>11</v>
       </c>
       <c r="I24" s="15">
-        <f t="shared" si="13"/>
+        <f>$A24+I$18</f>
         <v>12</v>
       </c>
       <c r="J24" s="13">
-        <f t="shared" si="13"/>
+        <f>$A24+J$18</f>
         <v>13</v>
       </c>
       <c r="K24" s="19">
@@ -2282,35 +2282,35 @@
         <v>5</v>
       </c>
       <c r="N24" s="12">
-        <f t="shared" si="14"/>
+        <f>$M24+N$18</f>
         <v>5</v>
       </c>
       <c r="O24" s="16">
-        <f t="shared" si="14"/>
+        <f>$M24+O$18</f>
         <v>6</v>
       </c>
       <c r="P24" s="12">
-        <f t="shared" si="14"/>
+        <f>$M24+P$18</f>
         <v>7</v>
       </c>
       <c r="Q24" s="16">
-        <f t="shared" si="14"/>
+        <f>$M24+Q$18</f>
         <v>8</v>
       </c>
       <c r="R24" s="12">
-        <f t="shared" si="14"/>
+        <f>$M24+R$18</f>
         <v>9</v>
       </c>
       <c r="S24" s="16">
-        <f t="shared" si="14"/>
+        <f>$M24+S$18</f>
         <v>10</v>
       </c>
       <c r="T24" s="12">
-        <f t="shared" si="14"/>
+        <f>$M24+T$18</f>
         <v>11</v>
       </c>
       <c r="U24" s="16">
-        <f t="shared" si="14"/>
+        <f>$M24+U$18</f>
         <v>12</v>
       </c>
       <c r="V24" s="20">
@@ -2323,39 +2323,39 @@
         <v>6</v>
       </c>
       <c r="B25" s="15">
-        <f t="shared" si="13"/>
+        <f>$A25+B$18</f>
         <v>6</v>
       </c>
       <c r="C25" s="13">
-        <f t="shared" si="13"/>
+        <f>$A25+C$18</f>
         <v>7</v>
       </c>
       <c r="D25" s="15">
-        <f t="shared" si="13"/>
+        <f>$A25+D$18</f>
         <v>8</v>
       </c>
       <c r="E25" s="13">
-        <f t="shared" si="13"/>
+        <f>$A25+E$18</f>
         <v>9</v>
       </c>
       <c r="F25" s="15">
-        <f t="shared" si="13"/>
+        <f>$A25+F$18</f>
         <v>10</v>
       </c>
       <c r="G25" s="13">
-        <f t="shared" si="13"/>
+        <f>$A25+G$18</f>
         <v>11</v>
       </c>
       <c r="H25" s="15">
-        <f t="shared" si="13"/>
+        <f>$A25+H$18</f>
         <v>12</v>
       </c>
       <c r="I25" s="13">
-        <f t="shared" si="13"/>
+        <f>$A25+I$18</f>
         <v>13</v>
       </c>
       <c r="J25" s="15">
-        <f t="shared" si="13"/>
+        <f>$A25+J$18</f>
         <v>14</v>
       </c>
       <c r="K25" s="20">
@@ -2366,35 +2366,35 @@
         <v>6</v>
       </c>
       <c r="N25" s="16">
-        <f t="shared" si="14"/>
+        <f>$M25+N$18</f>
         <v>6</v>
       </c>
       <c r="O25" s="12">
-        <f t="shared" si="14"/>
+        <f>$M25+O$18</f>
         <v>7</v>
       </c>
       <c r="P25" s="16">
-        <f t="shared" si="14"/>
+        <f>$M25+P$18</f>
         <v>8</v>
       </c>
       <c r="Q25" s="12">
-        <f t="shared" si="14"/>
+        <f>$M25+Q$18</f>
         <v>9</v>
       </c>
       <c r="R25" s="16">
-        <f t="shared" si="14"/>
+        <f>$M25+R$18</f>
         <v>10</v>
       </c>
       <c r="S25" s="12">
-        <f t="shared" si="14"/>
+        <f>$M25+S$18</f>
         <v>11</v>
       </c>
       <c r="T25" s="16">
-        <f t="shared" si="14"/>
+        <f>$M25+T$18</f>
         <v>12</v>
       </c>
       <c r="U25" s="12">
-        <f t="shared" si="14"/>
+        <f>$M25+U$18</f>
         <v>13</v>
       </c>
       <c r="V25" s="19">
@@ -2407,39 +2407,39 @@
         <v>7</v>
       </c>
       <c r="B26" s="13">
-        <f t="shared" si="13"/>
+        <f>$A26+B$18</f>
         <v>7</v>
       </c>
       <c r="C26" s="15">
-        <f t="shared" si="13"/>
+        <f>$A26+C$18</f>
         <v>8</v>
       </c>
       <c r="D26" s="13">
-        <f t="shared" si="13"/>
+        <f>$A26+D$18</f>
         <v>9</v>
       </c>
       <c r="E26" s="15">
-        <f t="shared" si="13"/>
+        <f>$A26+E$18</f>
         <v>10</v>
       </c>
       <c r="F26" s="13">
-        <f t="shared" si="13"/>
+        <f>$A26+F$18</f>
         <v>11</v>
       </c>
       <c r="G26" s="15">
-        <f t="shared" si="13"/>
+        <f>$A26+G$18</f>
         <v>12</v>
       </c>
       <c r="H26" s="13">
-        <f t="shared" si="13"/>
+        <f>$A26+H$18</f>
         <v>13</v>
       </c>
       <c r="I26" s="15">
-        <f t="shared" si="13"/>
+        <f>$A26+I$18</f>
         <v>14</v>
       </c>
       <c r="J26" s="13">
-        <f t="shared" si="13"/>
+        <f>$A26+J$18</f>
         <v>15</v>
       </c>
       <c r="K26" s="19">
@@ -2450,35 +2450,35 @@
         <v>7</v>
       </c>
       <c r="N26" s="12">
-        <f t="shared" si="14"/>
+        <f>$M26+N$18</f>
         <v>7</v>
       </c>
       <c r="O26" s="16">
-        <f t="shared" si="14"/>
+        <f>$M26+O$18</f>
         <v>8</v>
       </c>
       <c r="P26" s="12">
-        <f t="shared" si="14"/>
+        <f>$M26+P$18</f>
         <v>9</v>
       </c>
       <c r="Q26" s="16">
-        <f t="shared" si="14"/>
+        <f>$M26+Q$18</f>
         <v>10</v>
       </c>
       <c r="R26" s="12">
-        <f t="shared" si="14"/>
+        <f>$M26+R$18</f>
         <v>11</v>
       </c>
       <c r="S26" s="16">
-        <f t="shared" si="14"/>
+        <f>$M26+S$18</f>
         <v>12</v>
       </c>
       <c r="T26" s="12">
-        <f t="shared" si="14"/>
+        <f>$M26+T$18</f>
         <v>13</v>
       </c>
       <c r="U26" s="16">
-        <f t="shared" si="14"/>
+        <f>$M26+U$18</f>
         <v>14</v>
       </c>
       <c r="V26" s="20">
@@ -2491,39 +2491,39 @@
         <v>8</v>
       </c>
       <c r="B27" s="15">
-        <f t="shared" si="13"/>
+        <f>$A27+B$18</f>
         <v>8</v>
       </c>
       <c r="C27" s="13">
-        <f t="shared" si="13"/>
+        <f>$A27+C$18</f>
         <v>9</v>
       </c>
       <c r="D27" s="15">
-        <f t="shared" si="13"/>
+        <f>$A27+D$18</f>
         <v>10</v>
       </c>
       <c r="E27" s="13">
-        <f t="shared" si="13"/>
+        <f>$A27+E$18</f>
         <v>11</v>
       </c>
       <c r="F27" s="15">
-        <f t="shared" si="13"/>
+        <f>$A27+F$18</f>
         <v>12</v>
       </c>
       <c r="G27" s="13">
-        <f t="shared" si="13"/>
+        <f>$A27+G$18</f>
         <v>13</v>
       </c>
       <c r="H27" s="15">
-        <f t="shared" si="13"/>
+        <f>$A27+H$18</f>
         <v>14</v>
       </c>
       <c r="I27" s="13">
-        <f t="shared" si="13"/>
+        <f>$A27+I$18</f>
         <v>15</v>
       </c>
       <c r="J27" s="15">
-        <f t="shared" si="13"/>
+        <f>$A27+J$18</f>
         <v>16</v>
       </c>
       <c r="K27" s="20">

</xml_diff>